<commit_message>
class complete sequence drawing
</commit_message>
<xml_diff>
--- a/design/base_local_planner.xlsx
+++ b/design/base_local_planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C77911F-67C1-4B7A-A679-A4BF831360E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3D5311-C97F-4CAE-8DE0-9EF570626F32}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="327" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="327" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ソース一覧" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
   <si>
     <t>costmap_model.cpp</t>
     <phoneticPr fontId="1"/>
@@ -686,6 +686,29 @@
       <t>ズ</t>
     </rPh>
     <rPh sb="5" eb="6">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時間がかかるからやめたほうが良いことがわかった</t>
+    <rPh sb="0" eb="2">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>movebaseを見て、シーケンス図を書く</t>
+    <rPh sb="9" eb="10">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
       <t>カ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -746,11 +769,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1111,357 +1131,361 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="31.625" customWidth="1"/>
     <col min="2" max="2" width="38.25" customWidth="1"/>
-    <col min="3" max="3" width="16.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" style="1" customWidth="1"/>
     <col min="5" max="5" width="49.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>2</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>4</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>5</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>2</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>3</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>3</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>0</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>1</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>3</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>3</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>0</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>2</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>3</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>1</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>1</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>0</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>0</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>1</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>0</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="7">
         <v>0</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="7">
         <v>0</v>
       </c>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="7">
         <v>1</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="7">
         <v>1</v>
       </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>5</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>6</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="7">
         <v>0</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="7">
         <v>1</v>
       </c>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="7">
         <v>1</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="7">
         <v>1</v>
       </c>
+      <c r="E23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1484,9 +1508,9 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.625" customWidth="1"/>
-    <col min="2" max="2" width="31.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.75" customWidth="1"/>
-    <col min="4" max="4" width="25.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="3.75" customWidth="1"/>
     <col min="6" max="6" width="33.375" customWidth="1"/>
     <col min="7" max="7" width="3.25" customWidth="1"/>
@@ -1496,49 +1520,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F4" t="s">
@@ -1547,41 +1571,41 @@
       <c r="H4" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="D5" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J7" t="s">
@@ -1589,205 +1613,205 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F15" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F18" t="s">
         <v>112</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F20" t="s">
         <v>115</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>95</v>
       </c>
       <c r="F22" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1802,26 +1826,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="2"/>
+    <col min="1" max="1" width="8.75" style="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1829,7 +1853,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1840,7 +1864,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1848,7 +1872,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1861,7 +1885,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1869,106 +1893,112 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <f>A7+1</f>
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>120</v>
       </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <f t="shared" ref="A9:A24" si="0">A8+1</f>
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>

</xml_diff>